<commit_message>
Most up to date
</commit_message>
<xml_diff>
--- a/Te Ohange Chase Development Plan (version 1).xlsx
+++ b/Te Ohange Chase Development Plan (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\source\repos\TeOhangaChaseV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF732ACB-81E5-4174-A189-DE7BF773F379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2316AD58-F4DB-4278-BDCC-58FA11F97F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="705" windowWidth="19440" windowHeight="15000" xr2:uid="{F3A18A50-B025-4E36-B932-C8DA9519A223}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Te Ohange Chase Development Plan</t>
   </si>
@@ -88,6 +87,9 @@
   </si>
   <si>
     <t>Full Screen/minimise buttons</t>
+  </si>
+  <si>
+    <t>Only basic implementation</t>
   </si>
 </sst>
 </file>
@@ -165,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -177,6 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +502,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +510,7 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,8 +561,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="C6" s="9">
+        <v>43867</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>5</v>
@@ -575,8 +582,14 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="C8" s="9">
+        <v>43867</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>7</v>

</xml_diff>